<commit_message>
Bulletin de paie __ 5a et 7 et 10 et 11
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/6_Bulletin_De_Paies/Bulletin_De_Paie.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/6_Bulletin_De_Paies/Bulletin_De_Paie.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>BULLETIN DE PAIE</t>
   </si>
@@ -158,15 +158,9 @@
     <t>Au</t>
   </si>
   <si>
-    <t>SALAIRE BRUT</t>
-  </si>
-  <si>
     <t>Salarié</t>
   </si>
   <si>
-    <t xml:space="preserve">Retenues </t>
-  </si>
-  <si>
     <t>Base [€]</t>
   </si>
   <si>
@@ -303,18 +297,37 @@
   </si>
   <si>
     <t>1,30 </t>
+  </si>
+  <si>
+    <t>SALAIRE MENSUEL BRUT</t>
+  </si>
+  <si>
+    <t>Date de paiement du salaire</t>
+  </si>
+  <si>
+    <t>Nombre d'heures de travail</t>
+  </si>
+  <si>
+    <t>Nombre d'heures payées au taux normal (...€/heure)</t>
+  </si>
+  <si>
+    <t>Nombre d'heures supplémentaires payées à un taux spécifique (...€/heure)</t>
+  </si>
+  <si>
+    <t>Retenues ou accessoires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -533,7 +546,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -687,18 +700,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -782,6 +783,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,16 +1126,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U69"/>
+  <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="101.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1157,7 +1195,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:21" ht="75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1186,7 +1224,7 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:21" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
@@ -1215,7 +1253,7 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="1:21" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1282,7 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="243.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1311,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" ht="324" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="54" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1338,7 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:21" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1365,7 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:21" ht="36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -1674,8 +1712,10 @@
       <c r="U21" s="4"/>
     </row>
     <row r="22" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="69"/>
       <c r="C22" s="37"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -1695,16 +1735,20 @@
       <c r="U22" s="4"/>
     </row>
     <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="A23" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="72">
+        <f>SUM(B24:B25)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="37"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="38"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -1717,25 +1761,20 @@
       <c r="U23" s="4"/>
     </row>
     <row r="24" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="40">
-        <f>550</f>
-        <v>550</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="43"/>
+      <c r="A24" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="73">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="38"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
@@ -1748,28 +1787,20 @@
       <c r="U24" s="4"/>
     </row>
     <row r="25" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="45" t="s">
-        <v>38</v>
-      </c>
+      <c r="A25" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="74">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="38"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1782,28 +1813,12 @@
       <c r="U25" s="4"/>
     </row>
     <row r="26" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="40">
-        <f>$B$24*$B$50</f>
-        <v>540.375</v>
-      </c>
-      <c r="C26" s="47">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="40">
-        <f t="shared" ref="D26:D40" si="0">C26*B26</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="48">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="F26" s="40">
-        <f t="shared" ref="F26:F34" si="1">B26*E26</f>
-        <v>36.7455</v>
-      </c>
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="38"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1820,28 +1835,21 @@
       <c r="U26" s="4"/>
     </row>
     <row r="27" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
-        <v>40</v>
+      <c r="A27" s="39" t="s">
+        <v>79</v>
       </c>
       <c r="B27" s="40">
-        <f>$B$24*$B$50</f>
-        <v>540.375</v>
-      </c>
-      <c r="C27" s="47">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="48">
-        <v>2.4E-2</v>
-      </c>
-      <c r="F27" s="40">
-        <f t="shared" si="1"/>
-        <v>12.968999999999999</v>
-      </c>
+        <f>550</f>
+        <v>550</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="65"/>
+      <c r="E27" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="67"/>
       <c r="G27" s="38"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1858,27 +1866,23 @@
       <c r="U27" s="4"/>
     </row>
     <row r="28" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="40">
-        <f>$B$24*$B$50</f>
-        <v>540.375</v>
-      </c>
-      <c r="C28" s="49">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="48">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F28" s="40">
-        <f t="shared" si="1"/>
-        <v>2.7018750000000002</v>
+      <c r="A28" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>36</v>
       </c>
       <c r="G28" s="38"/>
       <c r="I28" s="4"/>
@@ -1896,26 +1900,27 @@
       <c r="U28" s="4"/>
     </row>
     <row r="29" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="46" t="s">
-        <v>42</v>
+      <c r="A29" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="B29" s="40">
-        <f t="shared" ref="B29:B40" si="2">$B$24</f>
-        <v>550</v>
-      </c>
-      <c r="C29" s="48">
-        <v>0.13</v>
+        <f>$B$27*$B$53</f>
+        <v>540.375</v>
+      </c>
+      <c r="C29" s="44">
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="D29" s="40">
-        <f t="shared" si="0"/>
-        <v>71.5</v>
-      </c>
-      <c r="E29" s="48">
-        <v>7.4999999999999997E-3</v>
+        <f t="shared" ref="D29:D43" si="0">C29*B29</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="45">
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F29" s="40">
-        <f t="shared" si="1"/>
-        <v>4.125</v>
+        <f t="shared" ref="F29:F37" si="1">B29*E29</f>
+        <v>36.7455</v>
       </c>
       <c r="G29" s="38"/>
       <c r="I29" s="4"/>
@@ -1933,36 +1938,37 @@
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="46" t="s">
-        <v>43</v>
+      <c r="A30" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="B30" s="40">
-        <f t="shared" si="2"/>
-        <v>550</v>
-      </c>
-      <c r="C30" s="48">
-        <v>8.5500000000000007E-2</v>
+        <f>$B$27*$B$53</f>
+        <v>540.375</v>
+      </c>
+      <c r="C30" s="44">
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="D30" s="40">
         <f t="shared" si="0"/>
-        <v>47.025000000000006</v>
-      </c>
-      <c r="E30" s="48">
-        <v>6.9000000000000006E-2</v>
+        <v>0</v>
+      </c>
+      <c r="E30" s="45">
+        <v>2.4E-2</v>
       </c>
       <c r="F30" s="40">
         <f t="shared" si="1"/>
-        <v>37.950000000000003</v>
+        <v>12.968999999999999</v>
       </c>
       <c r="G30" s="38"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -1970,35 +1976,37 @@
       <c r="U30" s="4"/>
     </row>
     <row r="31" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="46" t="s">
-        <v>44</v>
+      <c r="A31" s="43" t="s">
+        <v>39</v>
       </c>
       <c r="B31" s="40">
-        <f t="shared" si="2"/>
-        <v>550</v>
-      </c>
-      <c r="C31" s="48">
-        <v>1.9E-2</v>
+        <f>$B$27*$B$53</f>
+        <v>540.375</v>
+      </c>
+      <c r="C31" s="46">
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="D31" s="40">
         <f t="shared" si="0"/>
-        <v>10.45</v>
-      </c>
-      <c r="E31" s="48">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
+      </c>
+      <c r="E31" s="45">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F31" s="40">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.7018750000000002</v>
       </c>
       <c r="G31" s="38"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -2006,35 +2014,36 @@
       <c r="U31" s="4"/>
     </row>
     <row r="32" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
-        <v>45</v>
+      <c r="A32" s="43" t="s">
+        <v>40</v>
       </c>
       <c r="B32" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B32:B43" si="2">$B$27</f>
         <v>550</v>
       </c>
-      <c r="C32" s="48">
-        <v>3.1E-2</v>
+      <c r="C32" s="45">
+        <v>0.13</v>
       </c>
       <c r="D32" s="40">
         <f t="shared" si="0"/>
-        <v>17.05</v>
-      </c>
-      <c r="E32" s="48">
-        <v>4.7500000000000001E-2</v>
+        <v>71.5</v>
+      </c>
+      <c r="E32" s="45">
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F32" s="40">
         <f t="shared" si="1"/>
-        <v>26.125</v>
+        <v>4.125</v>
       </c>
       <c r="G32" s="38"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
@@ -2042,35 +2051,36 @@
       <c r="U32" s="4"/>
     </row>
     <row r="33" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="s">
-        <v>46</v>
+      <c r="A33" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="B33" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C33" s="48">
-        <v>4.0500000000000001E-2</v>
+      <c r="C33" s="45">
+        <v>8.5500000000000007E-2</v>
       </c>
       <c r="D33" s="40">
         <f t="shared" si="0"/>
-        <v>22.275000000000002</v>
-      </c>
-      <c r="E33" s="48">
-        <v>9.4999999999999998E-3</v>
+        <v>47.025000000000006</v>
+      </c>
+      <c r="E33" s="45">
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="F33" s="40">
         <f t="shared" si="1"/>
-        <v>5.2249999999999996</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="G33" s="38"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
@@ -2078,35 +2088,35 @@
       <c r="U33" s="4"/>
     </row>
     <row r="34" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>47</v>
+      <c r="A34" s="43" t="s">
+        <v>42</v>
       </c>
       <c r="B34" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C34" s="48">
-        <v>1.2E-2</v>
+      <c r="C34" s="45">
+        <v>1.9E-2</v>
       </c>
       <c r="D34" s="40">
         <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
-      </c>
-      <c r="E34" s="48">
-        <v>8.0000000000000002E-3</v>
+        <v>10.45</v>
+      </c>
+      <c r="E34" s="45">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F34" s="40">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G34" s="38"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
@@ -2114,33 +2124,35 @@
       <c r="U34" s="4"/>
     </row>
     <row r="35" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="46" t="s">
-        <v>48</v>
+      <c r="A35" s="43" t="s">
+        <v>43</v>
       </c>
       <c r="B35" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C35" s="48">
-        <v>5.2499999999999998E-2</v>
+      <c r="C35" s="45">
+        <v>3.1E-2</v>
       </c>
       <c r="D35" s="40">
         <f t="shared" si="0"/>
-        <v>28.875</v>
-      </c>
-      <c r="E35" s="48"/>
+        <v>17.05</v>
+      </c>
+      <c r="E35" s="45">
+        <v>4.7500000000000001E-2</v>
+      </c>
       <c r="F35" s="40">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>26.125</v>
       </c>
       <c r="G35" s="38"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
@@ -2148,33 +2160,35 @@
       <c r="U35" s="4"/>
     </row>
     <row r="36" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
-        <v>49</v>
+      <c r="A36" s="43" t="s">
+        <v>44</v>
       </c>
       <c r="B36" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C36" s="48">
-        <v>2.1000000000000001E-2</v>
+      <c r="C36" s="45">
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="D36" s="40">
         <f t="shared" si="0"/>
-        <v>11.55</v>
-      </c>
-      <c r="E36" s="48"/>
+        <v>22.275000000000002</v>
+      </c>
+      <c r="E36" s="45">
+        <v>9.4999999999999998E-3</v>
+      </c>
       <c r="F36" s="40">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.2249999999999996</v>
       </c>
       <c r="G36" s="38"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
@@ -2182,33 +2196,35 @@
       <c r="U36" s="4"/>
     </row>
     <row r="37" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
-        <v>50</v>
+      <c r="A37" s="43" t="s">
+        <v>45</v>
       </c>
       <c r="B37" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C37" s="48">
-        <v>1E-3</v>
+      <c r="C37" s="45">
+        <v>1.2E-2</v>
       </c>
       <c r="D37" s="40">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E37" s="48"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="E37" s="45">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="F37" s="40">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G37" s="38"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
+      <c r="P37" s="47"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
@@ -2216,36 +2232,33 @@
       <c r="U37" s="4"/>
     </row>
     <row r="38" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
-        <v>51</v>
+      <c r="A38" s="43" t="s">
+        <v>46</v>
       </c>
       <c r="B38" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C38" s="48">
-        <v>9.1000000000000004E-3</v>
+      <c r="C38" s="45">
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="D38" s="40">
         <f t="shared" si="0"/>
-        <v>5.0049999999999999</v>
-      </c>
-      <c r="E38" s="48">
-        <v>0</v>
-      </c>
+        <v>28.875</v>
+      </c>
+      <c r="E38" s="45"/>
       <c r="F38" s="40">
-        <f>E38*B38</f>
         <v>0</v>
       </c>
       <c r="G38" s="38"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="47"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
@@ -2253,22 +2266,24 @@
       <c r="U38" s="4"/>
     </row>
     <row r="39" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="46" t="s">
-        <v>52</v>
+      <c r="A39" s="43" t="s">
+        <v>47</v>
       </c>
       <c r="B39" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C39" s="48">
-        <v>3.5000000000000001E-3</v>
+      <c r="C39" s="45">
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D39" s="40">
         <f t="shared" si="0"/>
-        <v>1.925</v>
-      </c>
-      <c r="E39" s="48"/>
-      <c r="F39" s="40"/>
+        <v>11.55</v>
+      </c>
+      <c r="E39" s="45"/>
+      <c r="F39" s="40">
+        <v>0</v>
+      </c>
       <c r="G39" s="38"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -2285,22 +2300,24 @@
       <c r="U39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
-        <v>53</v>
+      <c r="A40" s="43" t="s">
+        <v>48</v>
       </c>
       <c r="B40" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
-      <c r="C40" s="48">
-        <v>3.0000000000000001E-3</v>
+      <c r="C40" s="45">
+        <v>1E-3</v>
       </c>
       <c r="D40" s="40">
         <f t="shared" si="0"/>
-        <v>1.6500000000000001</v>
-      </c>
-      <c r="E40" s="47"/>
-      <c r="F40" s="40"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E40" s="45"/>
+      <c r="F40" s="40">
+        <v>0</v>
+      </c>
       <c r="G40" s="38"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2317,19 +2334,32 @@
       <c r="U40" s="4"/>
     </row>
     <row r="41" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="40"/>
+      <c r="A41" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="40">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="C41" s="45">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="D41" s="40">
+        <f t="shared" si="0"/>
+        <v>5.0049999999999999</v>
+      </c>
+      <c r="E41" s="45">
+        <v>0</v>
+      </c>
+      <c r="F41" s="40">
+        <f>E41*B41</f>
+        <v>0</v>
+      </c>
       <c r="G41" s="38"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="51"/>
+      <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -2341,13 +2371,21 @@
       <c r="U41" s="4"/>
     </row>
     <row r="42" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="48"/>
+      <c r="A42" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="40">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="C42" s="45">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="D42" s="40">
+        <f t="shared" si="0"/>
+        <v>1.925</v>
+      </c>
+      <c r="E42" s="45"/>
       <c r="F42" s="40"/>
       <c r="G42" s="38"/>
       <c r="I42" s="4"/>
@@ -2365,13 +2403,21 @@
       <c r="U42" s="4"/>
     </row>
     <row r="43" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="48"/>
+      <c r="A43" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="40">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="C43" s="45">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D43" s="40">
+        <f t="shared" si="0"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="E43" s="44"/>
       <c r="F43" s="40"/>
       <c r="G43" s="38"/>
       <c r="I43" s="4"/>
@@ -2389,25 +2435,19 @@
       <c r="U43" s="4"/>
     </row>
     <row r="44" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="52">
-        <f>SUM(D29:D41)</f>
-        <v>224.45500000000004</v>
-      </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="52">
-        <f>SUM(F26:F41)</f>
-        <v>132.44137500000002</v>
-      </c>
+      <c r="A44" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="40"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="40"/>
       <c r="G44" s="38"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
+      <c r="L44" s="48"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -2419,17 +2459,14 @@
       <c r="U44" s="4"/>
     </row>
     <row r="45" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="52"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="52">
-        <f>B24-F44</f>
-        <v>417.55862500000001</v>
-      </c>
+      <c r="A45" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="40"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="40"/>
       <c r="G45" s="38"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2446,20 +2483,18 @@
       <c r="U45" s="4"/>
     </row>
     <row r="46" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="52"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="52">
-        <f>F45+F27+F28</f>
-        <v>433.22949999999997</v>
-      </c>
+      <c r="A46" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="40"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="40"/>
       <c r="G46" s="38"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -2472,14 +2507,20 @@
       <c r="U46" s="4"/>
     </row>
     <row r="47" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="52"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="56"/>
+      <c r="A47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="49">
+        <f>SUM(D32:D44)</f>
+        <v>224.45500000000004</v>
+      </c>
+      <c r="E47" s="50"/>
+      <c r="F47" s="49">
+        <f>SUM(F29:F44)</f>
+        <v>132.44137500000002</v>
+      </c>
       <c r="G47" s="38"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -2497,18 +2538,17 @@
     </row>
     <row r="48" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="52"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="52">
-        <f>F45</f>
+        <v>56</v>
+      </c>
+      <c r="B48" s="49"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="49">
+        <f>B27-F47</f>
         <v>417.55862500000001</v>
       </c>
-      <c r="G48" s="37"/>
-      <c r="H48" s="57"/>
+      <c r="G48" s="38"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -2523,20 +2563,21 @@
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
     </row>
-    <row r="49" spans="1:21" ht="288" x14ac:dyDescent="0.3">
-      <c r="A49" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="60"/>
+    <row r="49" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="49"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="49">
+        <f>F48+F30+F31</f>
+        <v>433.22949999999997</v>
+      </c>
+      <c r="G49" s="38"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
@@ -2549,18 +2590,15 @@
       <c r="U49" s="4"/>
     </row>
     <row r="50" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="62">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="A50" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="49"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="38"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -2576,14 +2614,19 @@
       <c r="U50" s="4"/>
     </row>
     <row r="51" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="4"/>
+      <c r="A51" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="49"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="49">
+        <f>F48</f>
+        <v>417.55862500000001</v>
+      </c>
+      <c r="G51" s="37"/>
+      <c r="H51" s="54"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -2598,25 +2641,17 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="1:21" ht="180" x14ac:dyDescent="0.3">
-      <c r="A52" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="65">
-        <v>7.75</v>
-      </c>
-      <c r="D52" s="65">
-        <v>3.1</v>
-      </c>
-      <c r="E52" s="65">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="4"/>
+    <row r="52" spans="1:21" ht="54" x14ac:dyDescent="0.3">
+      <c r="A52" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="22"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="57"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -2631,23 +2666,19 @@
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A53" s="65"/>
-      <c r="B53" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="65">
-        <v>2</v>
-      </c>
-      <c r="D53" s="65">
-        <v>0.8</v>
-      </c>
-      <c r="E53" s="65">
-        <v>1.2</v>
-      </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="4"/>
+    <row r="53" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="59">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="57"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -2662,22 +2693,14 @@
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="54" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A54" s="65"/>
-      <c r="B54" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="65">
-        <v>20.25</v>
-      </c>
-      <c r="D54" s="65">
-        <v>8.1</v>
-      </c>
-      <c r="E54" s="65">
-        <v>12.15</v>
-      </c>
+    <row r="54" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="22"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
       <c r="F54" s="22"/>
-      <c r="G54" s="64"/>
+      <c r="G54" s="61"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -2693,22 +2716,24 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
     </row>
-    <row r="55" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A55" s="65"/>
-      <c r="B55" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D55" s="65">
-        <v>0.9</v>
-      </c>
-      <c r="E55" s="65">
-        <v>1.3</v>
+    <row r="55" spans="1:21" ht="36" x14ac:dyDescent="0.3">
+      <c r="A55" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="62">
+        <v>7.75</v>
+      </c>
+      <c r="D55" s="62">
+        <v>3.1</v>
+      </c>
+      <c r="E55" s="62">
+        <v>4.6500000000000004</v>
       </c>
       <c r="F55" s="22"/>
-      <c r="G55" s="64"/>
+      <c r="G55" s="61"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -2725,13 +2750,21 @@
       <c r="U55" s="4"/>
     </row>
     <row r="56" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="65"/>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="65"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="62">
+        <v>2</v>
+      </c>
+      <c r="D56" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="E56" s="62">
+        <v>1.2</v>
+      </c>
       <c r="F56" s="22"/>
-      <c r="G56" s="64"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -2747,24 +2780,22 @@
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="1:21" ht="162" x14ac:dyDescent="0.3">
-      <c r="A57" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="65">
-        <v>7.75</v>
-      </c>
-      <c r="D57" s="65">
-        <v>3.1</v>
-      </c>
-      <c r="E57" s="65">
-        <v>4.6500000000000004</v>
+    <row r="57" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="62"/>
+      <c r="B57" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="62">
+        <v>20.25</v>
+      </c>
+      <c r="D57" s="62">
+        <v>8.1</v>
+      </c>
+      <c r="E57" s="62">
+        <v>12.15</v>
       </c>
       <c r="F57" s="22"/>
-      <c r="G57" s="64"/>
+      <c r="G57" s="61"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -2780,22 +2811,22 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A58" s="65"/>
-      <c r="B58" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" s="65">
-        <v>2</v>
-      </c>
-      <c r="D58" s="65">
-        <v>0.8</v>
-      </c>
-      <c r="E58" s="65">
-        <v>1.2</v>
+    <row r="58" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="62"/>
+      <c r="B58" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="62">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D58" s="62">
+        <v>0.9</v>
+      </c>
+      <c r="E58" s="62">
+        <v>1.3</v>
       </c>
       <c r="F58" s="22"/>
-      <c r="G58" s="64"/>
+      <c r="G58" s="61"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -2811,22 +2842,14 @@
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
     </row>
-    <row r="59" spans="1:21" ht="90" x14ac:dyDescent="0.3">
-      <c r="A59" s="65"/>
-      <c r="B59" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="65">
-        <v>20.55</v>
-      </c>
-      <c r="D59" s="65">
-        <v>7.8</v>
-      </c>
-      <c r="E59" s="65" t="s">
-        <v>73</v>
-      </c>
+    <row r="59" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="62"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
       <c r="F59" s="22"/>
-      <c r="G59" s="64"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -2842,22 +2865,24 @@
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A60" s="65"/>
-      <c r="B60" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D60" s="65">
-        <v>0.9</v>
-      </c>
-      <c r="E60" s="65">
-        <v>1.3</v>
+    <row r="60" spans="1:21" ht="36" x14ac:dyDescent="0.3">
+      <c r="A60" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="62">
+        <v>7.75</v>
+      </c>
+      <c r="D60" s="62">
+        <v>3.1</v>
+      </c>
+      <c r="E60" s="62">
+        <v>4.6500000000000004</v>
       </c>
       <c r="F60" s="22"/>
-      <c r="G60" s="64"/>
+      <c r="G60" s="61"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -2873,22 +2898,22 @@
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
     </row>
-    <row r="61" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A61" s="65"/>
-      <c r="B61" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" s="65">
-        <v>20.55</v>
-      </c>
-      <c r="D61" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" s="65" t="s">
-        <v>76</v>
+    <row r="61" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="62"/>
+      <c r="B61" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="62">
+        <v>2</v>
+      </c>
+      <c r="D61" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="E61" s="62">
+        <v>1.2</v>
       </c>
       <c r="F61" s="22"/>
-      <c r="G61" s="64"/>
+      <c r="G61" s="61"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -2904,22 +2929,22 @@
       <c r="T61" s="4"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A62" s="65"/>
-      <c r="B62" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="C62" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="E62" s="65" t="s">
-        <v>80</v>
+    <row r="62" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="62"/>
+      <c r="B62" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="62">
+        <v>20.55</v>
+      </c>
+      <c r="D62" s="62">
+        <v>7.8</v>
+      </c>
+      <c r="E62" s="62" t="s">
+        <v>71</v>
       </c>
       <c r="F62" s="22"/>
-      <c r="G62" s="64"/>
+      <c r="G62" s="61"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -2936,13 +2961,21 @@
       <c r="U62" s="4"/>
     </row>
     <row r="63" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="66"/>
-      <c r="B63" s="66"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="67"/>
+      <c r="A63" s="62"/>
+      <c r="B63" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="62">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D63" s="62">
+        <v>0.9</v>
+      </c>
+      <c r="E63" s="62">
+        <v>1.3</v>
+      </c>
+      <c r="F63" s="22"/>
+      <c r="G63" s="61"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -2959,13 +2992,21 @@
       <c r="U63" s="4"/>
     </row>
     <row r="64" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="66"/>
-      <c r="B64" s="66"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="67"/>
+      <c r="A64" s="62"/>
+      <c r="B64" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="62">
+        <v>20.55</v>
+      </c>
+      <c r="D64" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="22"/>
+      <c r="G64" s="61"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -2981,42 +3022,89 @@
       <c r="T64" s="4"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
+    <row r="65" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="62"/>
+      <c r="B65" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="F65" s="22"/>
+      <c r="G65" s="61"/>
       <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+    </row>
+    <row r="66" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="63"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+      <c r="U66" s="4"/>
+    </row>
+    <row r="67" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="63"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+    </row>
+    <row r="68" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3026,10 +3114,40 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
+    <row r="70" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1"/>
@@ -3037,5 +3155,6 @@
     <hyperlink ref="K6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mettre certains comptes imprimés italiques gras
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/6_Bulletin_De_Paies/Bulletin_De_Paie.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/6_Bulletin_De_Paies/Bulletin_De_Paie.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>BULLETIN DE PAIE</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Salarié</t>
   </si>
   <si>
-    <t>Base [€]</t>
-  </si>
-  <si>
     <t>Taux</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Vieillesse plafonnée</t>
   </si>
   <si>
-    <t>Vieillesse déplafonnée</t>
-  </si>
-  <si>
     <t>Retraite complémentaire *</t>
   </si>
   <si>
@@ -315,6 +309,15 @@
   </si>
   <si>
     <t>Retenues ou accessoires</t>
+  </si>
+  <si>
+    <t>Assiette de cotisation [€]</t>
+  </si>
+  <si>
+    <t>Cotisations de sécurité sociale</t>
+  </si>
+  <si>
+    <t>Assurance vieillesse déplafonnée (retraite du régime général)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +475,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +555,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -785,6 +794,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -797,26 +827,13 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1126,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U72"/>
+  <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1328,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" ht="54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +1355,7 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -1712,10 +1729,10 @@
       <c r="U21" s="4"/>
     </row>
     <row r="22" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="69"/>
+      <c r="A22" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="66"/>
       <c r="C22" s="37"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -1735,10 +1752,10 @@
       <c r="U22" s="4"/>
     </row>
     <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="72">
+      <c r="A23" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="69">
         <f>SUM(B24:B25)</f>
         <v>0</v>
       </c>
@@ -1761,10 +1778,10 @@
       <c r="U23" s="4"/>
     </row>
     <row r="24" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="73">
+      <c r="A24" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="70">
         <f>0</f>
         <v>0</v>
       </c>
@@ -1787,10 +1804,10 @@
       <c r="U24" s="4"/>
     </row>
     <row r="25" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="74">
+      <c r="A25" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="71">
         <f>0</f>
         <v>0</v>
       </c>
@@ -1836,20 +1853,20 @@
     </row>
     <row r="27" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" s="40">
         <f>550</f>
         <v>550</v>
       </c>
-      <c r="C27" s="65" t="s">
+      <c r="C27" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="66" t="s">
+      <c r="D27" s="72"/>
+      <c r="E27" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="67"/>
+      <c r="F27" s="74"/>
       <c r="G27" s="38"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1867,22 +1884,22 @@
     </row>
     <row r="28" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="D28" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="E28" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="42" t="s">
         <v>35</v>
-      </c>
-      <c r="E28" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>36</v>
       </c>
       <c r="G28" s="38"/>
       <c r="I28" s="4"/>
@@ -1900,28 +1917,14 @@
       <c r="U28" s="4"/>
     </row>
     <row r="29" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="40">
-        <f>$B$27*$B$53</f>
-        <v>540.375</v>
-      </c>
-      <c r="C29" s="44">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="40">
-        <f t="shared" ref="D29:D43" si="0">C29*B29</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="45">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="F29" s="40">
-        <f t="shared" ref="F29:F37" si="1">B29*E29</f>
-        <v>36.7455</v>
-      </c>
+      <c r="A29" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="76"/>
       <c r="G29" s="38"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1939,10 +1942,10 @@
     </row>
     <row r="30" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="40">
-        <f>$B$27*$B$53</f>
+        <f>$B$27*$B$54</f>
         <v>540.375</v>
       </c>
       <c r="C30" s="44">
@@ -1950,15 +1953,15 @@
         <v>0</v>
       </c>
       <c r="D30" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D30:D44" si="0">C30*B30</f>
         <v>0</v>
       </c>
       <c r="E30" s="45">
-        <v>2.4E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F30" s="40">
-        <f t="shared" si="1"/>
-        <v>12.968999999999999</v>
+        <f t="shared" ref="F30:F38" si="1">B30*E30</f>
+        <v>36.7455</v>
       </c>
       <c r="G30" s="38"/>
       <c r="I30" s="4"/>
@@ -1977,13 +1980,13 @@
     </row>
     <row r="31" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="40">
-        <f>$B$27*$B$53</f>
+        <f>$B$27*$B$54</f>
         <v>540.375</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="44">
         <f>0</f>
         <v>0</v>
       </c>
@@ -1992,11 +1995,11 @@
         <v>0</v>
       </c>
       <c r="E31" s="45">
-        <v>5.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F31" s="40">
         <f t="shared" si="1"/>
-        <v>2.7018750000000002</v>
+        <v>12.968999999999999</v>
       </c>
       <c r="G31" s="38"/>
       <c r="I31" s="4"/>
@@ -2015,25 +2018,26 @@
     </row>
     <row r="32" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="40">
-        <f t="shared" ref="B32:B43" si="2">$B$27</f>
-        <v>550</v>
-      </c>
-      <c r="C32" s="45">
-        <v>0.13</v>
+        <f>$B$27*$B$54</f>
+        <v>540.375</v>
+      </c>
+      <c r="C32" s="46">
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="D32" s="40">
         <f t="shared" si="0"/>
-        <v>71.5</v>
+        <v>0</v>
       </c>
       <c r="E32" s="45">
-        <v>7.4999999999999997E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F32" s="40">
         <f t="shared" si="1"/>
-        <v>4.125</v>
+        <v>2.7018750000000002</v>
       </c>
       <c r="G32" s="38"/>
       <c r="I32" s="4"/>
@@ -2052,25 +2056,25 @@
     </row>
     <row r="33" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B33:B44" si="2">$B$27</f>
         <v>550</v>
       </c>
       <c r="C33" s="45">
-        <v>8.5500000000000007E-2</v>
+        <v>0.13</v>
       </c>
       <c r="D33" s="40">
         <f t="shared" si="0"/>
-        <v>47.025000000000006</v>
+        <v>71.5</v>
       </c>
       <c r="E33" s="45">
-        <v>6.9000000000000006E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F33" s="40">
         <f t="shared" si="1"/>
-        <v>37.950000000000003</v>
+        <v>4.125</v>
       </c>
       <c r="G33" s="38"/>
       <c r="I33" s="4"/>
@@ -2089,25 +2093,25 @@
     </row>
     <row r="34" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C34" s="45">
-        <v>1.9E-2</v>
+        <v>8.5500000000000007E-2</v>
       </c>
       <c r="D34" s="40">
         <f t="shared" si="0"/>
-        <v>10.45</v>
+        <v>47.025000000000006</v>
       </c>
       <c r="E34" s="45">
-        <v>4.0000000000000001E-3</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="F34" s="40">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="G34" s="38"/>
       <c r="I34" s="4"/>
@@ -2125,25 +2129,25 @@
     </row>
     <row r="35" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B35" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C35" s="45">
-        <v>3.1E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D35" s="40">
         <f t="shared" si="0"/>
-        <v>17.05</v>
+        <v>10.45</v>
       </c>
       <c r="E35" s="45">
-        <v>4.7500000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F35" s="40">
         <f t="shared" si="1"/>
-        <v>26.125</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G35" s="38"/>
       <c r="I35" s="4"/>
@@ -2161,25 +2165,25 @@
     </row>
     <row r="36" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C36" s="45">
-        <v>4.0500000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D36" s="40">
         <f t="shared" si="0"/>
-        <v>22.275000000000002</v>
+        <v>17.05</v>
       </c>
       <c r="E36" s="45">
-        <v>9.4999999999999998E-3</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F36" s="40">
         <f t="shared" si="1"/>
-        <v>5.2249999999999996</v>
+        <v>26.125</v>
       </c>
       <c r="G36" s="38"/>
       <c r="I36" s="4"/>
@@ -2197,25 +2201,25 @@
     </row>
     <row r="37" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B37" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C37" s="45">
-        <v>1.2E-2</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="D37" s="40">
         <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
+        <v>22.275000000000002</v>
       </c>
       <c r="E37" s="45">
-        <v>8.0000000000000002E-3</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="F37" s="40">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>5.2249999999999996</v>
       </c>
       <c r="G37" s="38"/>
       <c r="I37" s="4"/>
@@ -2233,22 +2237,25 @@
     </row>
     <row r="38" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B38" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C38" s="45">
-        <v>5.2499999999999998E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D38" s="40">
         <f t="shared" si="0"/>
-        <v>28.875</v>
-      </c>
-      <c r="E38" s="45"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="E38" s="45">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="F38" s="40">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G38" s="38"/>
       <c r="I38" s="4"/>
@@ -2267,18 +2274,18 @@
     </row>
     <row r="39" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B39" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C39" s="45">
-        <v>2.1000000000000001E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="D39" s="40">
         <f t="shared" si="0"/>
-        <v>11.55</v>
+        <v>28.875</v>
       </c>
       <c r="E39" s="45"/>
       <c r="F39" s="40">
@@ -2301,18 +2308,18 @@
     </row>
     <row r="40" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B40" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C40" s="45">
-        <v>1E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D40" s="40">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>11.55</v>
       </c>
       <c r="E40" s="45"/>
       <c r="F40" s="40">
@@ -2335,24 +2342,21 @@
     </row>
     <row r="41" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B41" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C41" s="45">
-        <v>9.1000000000000004E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D41" s="40">
         <f t="shared" si="0"/>
-        <v>5.0049999999999999</v>
-      </c>
-      <c r="E41" s="45">
-        <v>0</v>
-      </c>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E41" s="45"/>
       <c r="F41" s="40">
-        <f>E41*B41</f>
         <v>0</v>
       </c>
       <c r="G41" s="38"/>
@@ -2372,21 +2376,26 @@
     </row>
     <row r="42" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B42" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C42" s="45">
-        <v>3.5000000000000001E-3</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="D42" s="40">
         <f t="shared" si="0"/>
-        <v>1.925</v>
-      </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="40"/>
+        <v>5.0049999999999999</v>
+      </c>
+      <c r="E42" s="45">
+        <v>0</v>
+      </c>
+      <c r="F42" s="40">
+        <f>E42*B42</f>
+        <v>0</v>
+      </c>
       <c r="G42" s="38"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2404,20 +2413,20 @@
     </row>
     <row r="43" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B43" s="40">
         <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C43" s="45">
-        <v>3.0000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D43" s="40">
         <f t="shared" si="0"/>
-        <v>1.6500000000000001</v>
-      </c>
-      <c r="E43" s="44"/>
+        <v>1.925</v>
+      </c>
+      <c r="E43" s="45"/>
       <c r="F43" s="40"/>
       <c r="G43" s="38"/>
       <c r="I43" s="4"/>
@@ -2436,12 +2445,20 @@
     </row>
     <row r="44" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="45"/>
+        <v>49</v>
+      </c>
+      <c r="B44" s="40">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="C44" s="45">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D44" s="40">
+        <f t="shared" si="0"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="E44" s="44"/>
       <c r="F44" s="40"/>
       <c r="G44" s="38"/>
       <c r="I44" s="4"/>
@@ -2460,7 +2477,7 @@
     </row>
     <row r="45" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B45" s="40"/>
       <c r="C45" s="45"/>
@@ -2484,7 +2501,7 @@
     </row>
     <row r="46" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="43" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B46" s="40"/>
       <c r="C46" s="45"/>
@@ -2507,20 +2524,14 @@
       <c r="U46" s="4"/>
     </row>
     <row r="47" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="49"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="49">
-        <f>SUM(D32:D44)</f>
-        <v>224.45500000000004</v>
-      </c>
-      <c r="E47" s="50"/>
-      <c r="F47" s="49">
-        <f>SUM(F29:F44)</f>
-        <v>132.44137500000002</v>
-      </c>
+      <c r="A47" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="40"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="40"/>
       <c r="G47" s="38"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -2538,15 +2549,18 @@
     </row>
     <row r="48" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48" s="49"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="51"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="49">
+        <f>SUM(D33:D45)</f>
+        <v>224.45500000000004</v>
+      </c>
+      <c r="E48" s="50"/>
       <c r="F48" s="49">
-        <f>B27-F47</f>
-        <v>417.55862500000001</v>
+        <f>SUM(F30:F45)</f>
+        <v>132.44137500000002</v>
       </c>
       <c r="G48" s="38"/>
       <c r="I48" s="4"/>
@@ -2565,15 +2579,15 @@
     </row>
     <row r="49" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B49" s="49"/>
-      <c r="C49" s="50"/>
+      <c r="C49" s="51"/>
       <c r="D49" s="49"/>
       <c r="E49" s="51"/>
       <c r="F49" s="49">
-        <f>F48+F30+F31</f>
-        <v>433.22949999999997</v>
+        <f>B27-F48</f>
+        <v>417.55862500000001</v>
       </c>
       <c r="G49" s="38"/>
       <c r="I49" s="4"/>
@@ -2590,14 +2604,17 @@
       <c r="U49" s="4"/>
     </row>
     <row r="50" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="52" t="s">
-        <v>58</v>
+      <c r="A50" s="39" t="s">
+        <v>55</v>
       </c>
       <c r="B50" s="49"/>
-      <c r="C50" s="51"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="49"/>
       <c r="E50" s="51"/>
-      <c r="F50" s="53"/>
+      <c r="F50" s="49">
+        <f>F49+F31+F32</f>
+        <v>433.22949999999997</v>
+      </c>
       <c r="G50" s="38"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -2614,17 +2631,14 @@
       <c r="U50" s="4"/>
     </row>
     <row r="51" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="39" t="s">
-        <v>59</v>
+      <c r="A51" s="52" t="s">
+        <v>56</v>
       </c>
       <c r="B51" s="49"/>
-      <c r="C51" s="39"/>
+      <c r="C51" s="51"/>
       <c r="D51" s="49"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="49">
-        <f>F48</f>
-        <v>417.55862500000001</v>
-      </c>
+      <c r="E51" s="51"/>
+      <c r="F51" s="53"/>
       <c r="G51" s="37"/>
       <c r="H51" s="54"/>
       <c r="I51" s="4"/>
@@ -2641,15 +2655,18 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="1:21" ht="54" x14ac:dyDescent="0.3">
-      <c r="A52" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
+    <row r="52" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="49"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="49">
+        <f>F49</f>
+        <v>417.55862500000001</v>
+      </c>
       <c r="G52" s="56"/>
       <c r="H52" s="57"/>
       <c r="I52" s="4"/>
@@ -2667,16 +2684,14 @@
       <c r="U52" s="4"/>
     </row>
     <row r="53" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="59">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
+      <c r="A53" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
       <c r="G53" s="56"/>
       <c r="H53" s="57"/>
       <c r="I53" s="4"/>
@@ -2694,12 +2709,16 @@
       <c r="U53" s="4"/>
     </row>
     <row r="54" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
-      <c r="B54" s="37"/>
+      <c r="A54" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="59">
+        <v>0.98250000000000004</v>
+      </c>
       <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
       <c r="G54" s="61"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2716,22 +2735,12 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
     </row>
-    <row r="55" spans="1:21" ht="36" x14ac:dyDescent="0.3">
-      <c r="A55" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="62">
-        <v>7.75</v>
-      </c>
-      <c r="D55" s="62">
-        <v>3.1</v>
-      </c>
-      <c r="E55" s="62">
-        <v>4.6500000000000004</v>
-      </c>
+    <row r="55" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="22"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
       <c r="F55" s="22"/>
       <c r="G55" s="61"/>
       <c r="H55" s="4"/>
@@ -2750,18 +2759,20 @@
       <c r="U55" s="4"/>
     </row>
     <row r="56" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="62"/>
+      <c r="A56" s="62" t="s">
+        <v>60</v>
+      </c>
       <c r="B56" s="62" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C56" s="62">
-        <v>2</v>
+        <v>7.75</v>
       </c>
       <c r="D56" s="62">
-        <v>0.8</v>
+        <v>3.1</v>
       </c>
       <c r="E56" s="62">
-        <v>1.2</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F56" s="22"/>
       <c r="G56" s="61"/>
@@ -2783,16 +2794,16 @@
     <row r="57" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="62"/>
       <c r="B57" s="62" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C57" s="62">
-        <v>20.25</v>
+        <v>2</v>
       </c>
       <c r="D57" s="62">
-        <v>8.1</v>
+        <v>0.8</v>
       </c>
       <c r="E57" s="62">
-        <v>12.15</v>
+        <v>1.2</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="61"/>
@@ -2814,16 +2825,16 @@
     <row r="58" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="62"/>
       <c r="B58" s="62" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58" s="62">
-        <v>2.2000000000000002</v>
+        <v>20.25</v>
       </c>
       <c r="D58" s="62">
-        <v>0.9</v>
+        <v>8.1</v>
       </c>
       <c r="E58" s="62">
-        <v>1.3</v>
+        <v>12.15</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="61"/>
@@ -2844,10 +2855,18 @@
     </row>
     <row r="59" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="62"/>
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
+      <c r="B59" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="62">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D59" s="62">
+        <v>0.9</v>
+      </c>
+      <c r="E59" s="62">
+        <v>1.3</v>
+      </c>
       <c r="F59" s="22"/>
       <c r="G59" s="61"/>
       <c r="H59" s="4"/>
@@ -2865,22 +2884,12 @@
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="1:21" ht="36" x14ac:dyDescent="0.3">
-      <c r="A60" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="62">
-        <v>7.75</v>
-      </c>
-      <c r="D60" s="62">
-        <v>3.1</v>
-      </c>
-      <c r="E60" s="62">
-        <v>4.6500000000000004</v>
-      </c>
+    <row r="60" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="62"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
       <c r="F60" s="22"/>
       <c r="G60" s="61"/>
       <c r="H60" s="4"/>
@@ -2899,18 +2908,20 @@
       <c r="U60" s="4"/>
     </row>
     <row r="61" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="62"/>
+      <c r="A61" s="62" t="s">
+        <v>65</v>
+      </c>
       <c r="B61" s="62" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C61" s="62">
-        <v>2</v>
+        <v>7.75</v>
       </c>
       <c r="D61" s="62">
-        <v>0.8</v>
+        <v>3.1</v>
       </c>
       <c r="E61" s="62">
-        <v>1.2</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F61" s="22"/>
       <c r="G61" s="61"/>
@@ -2932,16 +2943,16 @@
     <row r="62" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="62"/>
       <c r="B62" s="62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C62" s="62">
-        <v>20.55</v>
+        <v>2</v>
       </c>
       <c r="D62" s="62">
-        <v>7.8</v>
-      </c>
-      <c r="E62" s="62" t="s">
-        <v>71</v>
+        <v>0.8</v>
+      </c>
+      <c r="E62" s="62">
+        <v>1.2</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="61"/>
@@ -2963,16 +2974,16 @@
     <row r="63" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="62"/>
       <c r="B63" s="62" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C63" s="62">
-        <v>2.2000000000000002</v>
+        <v>20.55</v>
       </c>
       <c r="D63" s="62">
-        <v>0.9</v>
-      </c>
-      <c r="E63" s="62">
-        <v>1.3</v>
+        <v>7.8</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>69</v>
       </c>
       <c r="F63" s="22"/>
       <c r="G63" s="61"/>
@@ -2994,16 +3005,16 @@
     <row r="64" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="62"/>
       <c r="B64" s="62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C64" s="62">
-        <v>20.55</v>
-      </c>
-      <c r="D64" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>74</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D64" s="62">
+        <v>0.9</v>
+      </c>
+      <c r="E64" s="62">
+        <v>1.3</v>
       </c>
       <c r="F64" s="22"/>
       <c r="G64" s="61"/>
@@ -3025,16 +3036,16 @@
     <row r="65" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="62"/>
       <c r="B65" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="62" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="C65" s="62">
+        <v>20.55</v>
       </c>
       <c r="D65" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="E65" s="62" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="61"/>
@@ -3054,12 +3065,20 @@
       <c r="U65" s="4"/>
     </row>
     <row r="66" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="63"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
+      <c r="A66" s="62"/>
+      <c r="B66" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="F66" s="22"/>
       <c r="G66" s="64"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -3100,16 +3119,16 @@
       <c r="U67" s="4"/>
     </row>
     <row r="68" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F68" s="4"/>
+      <c r="A68" s="63"/>
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -3143,6 +3162,14 @@
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>